<commit_message>
kati 1 katet done
</commit_message>
<xml_diff>
--- a/706-3-Slivove-Asllani-leg/3-Katet/regjistri/29-Koordinatat-e-kateve-706-3-Slivove-Asllani-leg.xlsx
+++ b/706-3-Slivove-Asllani-leg/3-Katet/regjistri/29-Koordinatat-e-kateve-706-3-Slivove-Asllani-leg.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Ferizaj\Slivovë\KADASTRALE\Agoni-Slivovë\706-3-Slivove-Asllani-leg\3-Katet\regjistri\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
@@ -10,9 +15,9 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$K$55</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$K$62</definedName>
   </definedNames>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="20">
   <si>
     <t>Y</t>
   </si>
@@ -97,7 +102,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -496,6 +501,72 @@
     <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -525,72 +596,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -629,7 +634,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{0F399456-FFFA-4806-B53B-2B24D3A1E278}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0F399456-FFFA-4806-B53B-2B24D3A1E278}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -685,7 +690,7 @@
         <xdr:cNvPr id="4" name="TextBox 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E91F6037-E9CB-49EA-8E58-E0677C590B64}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E91F6037-E9CB-49EA-8E58-E0677C590B64}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -746,7 +751,7 @@
         <xdr:cNvPr id="5" name="TextBox 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{07937452-2E79-4669-8F05-2069DFF859A1}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{07937452-2E79-4669-8F05-2069DFF859A1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -807,7 +812,7 @@
         <xdr:cNvPr id="6" name="TextBox 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{AD9F1684-A2E1-4EF0-89C9-1E368E9A0FDD}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AD9F1684-A2E1-4EF0-89C9-1E368E9A0FDD}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -882,7 +887,7 @@
         <xdr:cNvPr id="7" name="TextBox 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{87D2CC83-FE69-4C93-84EB-099D36DB81C5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{87D2CC83-FE69-4C93-84EB-099D36DB81C5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1222,7 +1227,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1230,10 +1235,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K58"/>
+  <dimension ref="A1:K65"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A4" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A34" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
+      <selection activeCell="L19" sqref="L19:Q47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1249,115 +1254,115 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="16"/>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
-      <c r="J1" s="16"/>
-      <c r="K1" s="16"/>
+      <c r="A1" s="38"/>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
+      <c r="I1" s="38"/>
+      <c r="J1" s="38"/>
+      <c r="K1" s="38"/>
     </row>
     <row r="2" spans="1:11" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="16"/>
-      <c r="B2" s="16"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
-      <c r="I2" s="16"/>
-      <c r="J2" s="16"/>
-      <c r="K2" s="16"/>
+      <c r="A2" s="38"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="38"/>
+      <c r="K2" s="38"/>
     </row>
     <row r="3" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="31" t="s">
+      <c r="A3" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="31"/>
-      <c r="C3" s="31"/>
-      <c r="D3" s="31"/>
-      <c r="E3" s="31"/>
-      <c r="F3" s="31"/>
-      <c r="G3" s="31"/>
-      <c r="H3" s="31"/>
-      <c r="I3" s="31"/>
-      <c r="J3" s="31"/>
-      <c r="K3" s="31"/>
+      <c r="B3" s="20"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="20"/>
+      <c r="H3" s="20"/>
+      <c r="I3" s="20"/>
+      <c r="J3" s="20"/>
+      <c r="K3" s="20"/>
     </row>
     <row r="4" spans="1:11" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="31"/>
-      <c r="B4" s="31"/>
-      <c r="C4" s="31"/>
-      <c r="D4" s="31"/>
-      <c r="E4" s="31"/>
-      <c r="F4" s="31"/>
-      <c r="G4" s="31"/>
-      <c r="H4" s="31"/>
-      <c r="I4" s="31"/>
-      <c r="J4" s="31"/>
-      <c r="K4" s="31"/>
+      <c r="A4" s="20"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="20"/>
+      <c r="K4" s="20"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="31"/>
-      <c r="B5" s="31"/>
-      <c r="C5" s="31"/>
-      <c r="D5" s="31"/>
-      <c r="E5" s="31"/>
-      <c r="F5" s="31"/>
-      <c r="G5" s="31"/>
-      <c r="H5" s="31"/>
-      <c r="I5" s="31"/>
-      <c r="J5" s="31"/>
-      <c r="K5" s="31"/>
+      <c r="A5" s="20"/>
+      <c r="B5" s="20"/>
+      <c r="C5" s="20"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="20"/>
+      <c r="F5" s="20"/>
+      <c r="G5" s="20"/>
+      <c r="H5" s="20"/>
+      <c r="I5" s="20"/>
+      <c r="J5" s="20"/>
+      <c r="K5" s="20"/>
     </row>
     <row r="6" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="31"/>
-      <c r="B6" s="31"/>
-      <c r="C6" s="31"/>
-      <c r="D6" s="31"/>
-      <c r="E6" s="31"/>
-      <c r="F6" s="31"/>
-      <c r="G6" s="31"/>
-      <c r="H6" s="31"/>
-      <c r="I6" s="31"/>
-      <c r="J6" s="31"/>
-      <c r="K6" s="31"/>
+      <c r="A6" s="20"/>
+      <c r="B6" s="20"/>
+      <c r="C6" s="20"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="20"/>
+      <c r="F6" s="20"/>
+      <c r="G6" s="20"/>
+      <c r="H6" s="20"/>
+      <c r="I6" s="20"/>
+      <c r="J6" s="20"/>
+      <c r="K6" s="20"/>
     </row>
     <row r="7" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C8" s="17"/>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="18"/>
-      <c r="H8" s="18"/>
-      <c r="I8" s="18"/>
-      <c r="J8" s="19"/>
+      <c r="C8" s="39"/>
+      <c r="D8" s="40"/>
+      <c r="E8" s="40"/>
+      <c r="F8" s="40"/>
+      <c r="G8" s="40"/>
+      <c r="H8" s="40"/>
+      <c r="I8" s="40"/>
+      <c r="J8" s="41"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C9" s="20"/>
-      <c r="D9" s="21"/>
-      <c r="E9" s="21"/>
-      <c r="F9" s="21"/>
-      <c r="G9" s="21"/>
-      <c r="H9" s="21"/>
-      <c r="I9" s="21"/>
-      <c r="J9" s="22"/>
+      <c r="C9" s="42"/>
+      <c r="D9" s="43"/>
+      <c r="E9" s="43"/>
+      <c r="F9" s="43"/>
+      <c r="G9" s="43"/>
+      <c r="H9" s="43"/>
+      <c r="I9" s="43"/>
+      <c r="J9" s="44"/>
     </row>
     <row r="10" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C10" s="23"/>
-      <c r="D10" s="24"/>
-      <c r="E10" s="24"/>
-      <c r="F10" s="24"/>
-      <c r="G10" s="24"/>
-      <c r="H10" s="24"/>
-      <c r="I10" s="24"/>
-      <c r="J10" s="25"/>
+      <c r="C10" s="45"/>
+      <c r="D10" s="46"/>
+      <c r="E10" s="46"/>
+      <c r="F10" s="46"/>
+      <c r="G10" s="46"/>
+      <c r="H10" s="46"/>
+      <c r="I10" s="46"/>
+      <c r="J10" s="47"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D12" s="4"/>
@@ -1409,13 +1414,13 @@
       <c r="F15" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="G15" s="26" t="s">
+      <c r="G15" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="H15" s="45" t="s">
+      <c r="H15" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="I15" s="45">
+      <c r="I15" s="35">
         <v>107.41</v>
       </c>
     </row>
@@ -1435,9 +1440,9 @@
       <c r="F16" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="G16" s="26"/>
-      <c r="H16" s="46"/>
-      <c r="I16" s="46"/>
+      <c r="G16" s="34"/>
+      <c r="H16" s="36"/>
+      <c r="I16" s="36"/>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B17" s="11">
@@ -1455,9 +1460,9 @@
       <c r="F17" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="G17" s="26"/>
-      <c r="H17" s="46"/>
-      <c r="I17" s="46"/>
+      <c r="G17" s="34"/>
+      <c r="H17" s="36"/>
+      <c r="I17" s="36"/>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B18" s="11">
@@ -1475,9 +1480,9 @@
       <c r="F18" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="G18" s="26"/>
-      <c r="H18" s="46"/>
-      <c r="I18" s="46"/>
+      <c r="G18" s="34"/>
+      <c r="H18" s="36"/>
+      <c r="I18" s="36"/>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B19" s="11">
@@ -1495,9 +1500,9 @@
       <c r="F19" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="G19" s="26"/>
-      <c r="H19" s="46"/>
-      <c r="I19" s="46"/>
+      <c r="G19" s="34"/>
+      <c r="H19" s="36"/>
+      <c r="I19" s="36"/>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B20" s="11">
@@ -1515,9 +1520,9 @@
       <c r="F20" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="G20" s="26"/>
-      <c r="H20" s="46"/>
-      <c r="I20" s="46"/>
+      <c r="G20" s="34"/>
+      <c r="H20" s="36"/>
+      <c r="I20" s="36"/>
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B21" s="11">
@@ -1535,9 +1540,9 @@
       <c r="F21" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="G21" s="26"/>
-      <c r="H21" s="46"/>
-      <c r="I21" s="46"/>
+      <c r="G21" s="34"/>
+      <c r="H21" s="36"/>
+      <c r="I21" s="36"/>
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B22" s="11">
@@ -1555,9 +1560,9 @@
       <c r="F22" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="G22" s="26"/>
-      <c r="H22" s="46"/>
-      <c r="I22" s="46"/>
+      <c r="G22" s="34"/>
+      <c r="H22" s="36"/>
+      <c r="I22" s="36"/>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B23" s="11">
@@ -1575,9 +1580,9 @@
       <c r="F23" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="G23" s="26"/>
-      <c r="H23" s="46"/>
-      <c r="I23" s="46"/>
+      <c r="G23" s="34"/>
+      <c r="H23" s="36"/>
+      <c r="I23" s="36"/>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B24" s="11">
@@ -1595,9 +1600,9 @@
       <c r="F24" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="G24" s="26"/>
-      <c r="H24" s="46"/>
-      <c r="I24" s="46"/>
+      <c r="G24" s="34"/>
+      <c r="H24" s="36"/>
+      <c r="I24" s="36"/>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B25" s="11">
@@ -1615,9 +1620,9 @@
       <c r="F25" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="G25" s="26"/>
-      <c r="H25" s="46"/>
-      <c r="I25" s="46"/>
+      <c r="G25" s="34"/>
+      <c r="H25" s="36"/>
+      <c r="I25" s="36"/>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B26" s="11">
@@ -1635,9 +1640,9 @@
       <c r="F26" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="G26" s="26"/>
-      <c r="H26" s="46"/>
-      <c r="I26" s="46"/>
+      <c r="G26" s="34"/>
+      <c r="H26" s="36"/>
+      <c r="I26" s="36"/>
     </row>
     <row r="27" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B27" s="11">
@@ -1655,9 +1660,9 @@
       <c r="F27" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="G27" s="26"/>
-      <c r="H27" s="46"/>
-      <c r="I27" s="46"/>
+      <c r="G27" s="34"/>
+      <c r="H27" s="36"/>
+      <c r="I27" s="36"/>
     </row>
     <row r="28" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B28" s="11">
@@ -1675,9 +1680,9 @@
       <c r="F28" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="G28" s="26"/>
-      <c r="H28" s="47"/>
-      <c r="I28" s="47"/>
+      <c r="G28" s="34"/>
+      <c r="H28" s="37"/>
+      <c r="I28" s="37"/>
     </row>
     <row r="29" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B29" s="11">
@@ -1695,7 +1700,7 @@
       <c r="F29" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="G29" s="26"/>
+      <c r="G29" s="34"/>
       <c r="H29" s="15" t="s">
         <v>13</v>
       </c>
@@ -1748,214 +1753,298 @@
     </row>
     <row r="33" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B33" s="11">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="C33" s="5">
-        <v>7512912.8032999998</v>
+        <v>7508327.6256999997</v>
       </c>
       <c r="D33" s="5">
-        <v>4688202.5635000002</v>
+        <v>4696771.6880000001</v>
       </c>
       <c r="E33" s="10">
-        <v>604.78599999999994</v>
+        <v>609.58299999999997</v>
       </c>
       <c r="F33" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="G33" s="26" t="s">
+      <c r="G33" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="H33" s="26" t="s">
+      <c r="H33" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="I33" s="26">
-        <v>78.774000000000001</v>
+      <c r="I33" s="34">
+        <v>87.864999999999995</v>
       </c>
     </row>
     <row r="34" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B34" s="11">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="C34" s="5">
-        <v>7512912.7340000002</v>
+        <v>7508329.2152000004</v>
       </c>
       <c r="D34" s="5">
-        <v>4688191.807</v>
+        <v>4696780.3870000001</v>
       </c>
       <c r="E34" s="10">
-        <v>604.78599999999994</v>
+        <v>609.58299999999997</v>
       </c>
       <c r="F34" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="G34" s="26"/>
-      <c r="H34" s="26"/>
-      <c r="I34" s="26"/>
+      <c r="G34" s="34"/>
+      <c r="H34" s="34"/>
+      <c r="I34" s="34"/>
     </row>
     <row r="35" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B35" s="11">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="C35" s="5">
-        <v>7512912.3449999997</v>
+        <v>7508338.3417999996</v>
       </c>
       <c r="D35" s="5">
-        <v>4688192.7699999996</v>
+        <v>4696778.6058999998</v>
       </c>
       <c r="E35" s="10">
-        <v>604.78599999999994</v>
+        <v>609.58299999999997</v>
       </c>
       <c r="F35" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="G35" s="26"/>
-      <c r="H35" s="26"/>
-      <c r="I35" s="26"/>
+      <c r="G35" s="34"/>
+      <c r="H35" s="34"/>
+      <c r="I35" s="34"/>
     </row>
     <row r="36" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B36" s="11">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="C36" s="5">
-        <v>7512908.3671000004</v>
+        <v>7508327.5800999999</v>
       </c>
       <c r="D36" s="5">
-        <v>4688191.2390000001</v>
+        <v>4696776.3726000004</v>
       </c>
       <c r="E36" s="10">
-        <v>604.78599999999994</v>
+        <v>609.58299999999997</v>
       </c>
       <c r="F36" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="G36" s="26"/>
-      <c r="H36" s="26"/>
-      <c r="I36" s="26"/>
+      <c r="G36" s="34"/>
+      <c r="H36" s="34"/>
+      <c r="I36" s="34"/>
     </row>
     <row r="37" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B37" s="11">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="C37" s="5">
-        <v>7512905.0429999996</v>
+        <v>7508327.1117000002</v>
       </c>
       <c r="D37" s="5">
-        <v>4688199.4000000004</v>
+        <v>4696773.8236999996</v>
       </c>
       <c r="E37" s="10">
-        <v>604.78599999999994</v>
+        <v>609.58299999999997</v>
       </c>
       <c r="F37" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="G37" s="26"/>
-      <c r="H37" s="26"/>
-      <c r="I37" s="26"/>
+      <c r="G37" s="34"/>
+      <c r="H37" s="34"/>
+      <c r="I37" s="34"/>
     </row>
     <row r="38" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B38" s="11">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C38" s="5">
-        <v>7512916.5610999996</v>
+        <v>7508327.9957999997</v>
       </c>
       <c r="D38" s="5">
-        <v>4688193.3693000004</v>
+        <v>4696773.6736000003</v>
       </c>
       <c r="E38" s="10">
-        <v>604.78599999999994</v>
+        <v>609.58299999999997</v>
       </c>
       <c r="F38" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="G38" s="26"/>
-      <c r="H38" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="I38" s="10">
-        <v>4.4909999999999997</v>
-      </c>
+      <c r="G38" s="34"/>
+      <c r="H38" s="34"/>
+      <c r="I38" s="34"/>
     </row>
     <row r="39" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B39" s="11">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C39" s="5">
-        <v>7512908.7709999997</v>
+        <v>7508328.4636000004</v>
       </c>
       <c r="D39" s="5">
-        <v>4688190.2439999999</v>
+        <v>4696776.2134999996</v>
       </c>
       <c r="E39" s="10">
-        <v>604.78599999999994</v>
+        <v>609.58299999999997</v>
       </c>
       <c r="F39" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="G39" s="34"/>
+      <c r="H39" s="34"/>
+      <c r="I39" s="34"/>
+    </row>
+    <row r="40" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B40" s="11">
+        <v>29</v>
+      </c>
+      <c r="C40" s="5">
+        <v>7508331.7936000004</v>
+      </c>
+      <c r="D40" s="5">
+        <v>4696770.8948999997</v>
+      </c>
+      <c r="E40" s="10">
+        <v>609.58299999999997</v>
+      </c>
+      <c r="F40" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="G40" s="34"/>
+      <c r="H40" s="34"/>
+      <c r="I40" s="34"/>
+    </row>
+    <row r="41" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B41" s="11">
+        <v>30</v>
+      </c>
+      <c r="C41" s="5">
+        <v>7508332.2145999996</v>
+      </c>
+      <c r="D41" s="5">
+        <v>4696770.6380000003</v>
+      </c>
+      <c r="E41" s="10">
+        <v>609.58299999999997</v>
+      </c>
+      <c r="F41" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="G41" s="34"/>
+      <c r="H41" s="34"/>
+      <c r="I41" s="34"/>
+    </row>
+    <row r="42" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B42" s="11">
+        <v>31</v>
+      </c>
+      <c r="C42" s="5">
+        <v>7508333.1083000004</v>
+      </c>
+      <c r="D42" s="5">
+        <v>4696769.4139</v>
+      </c>
+      <c r="E42" s="10">
+        <v>609.58299999999997</v>
+      </c>
+      <c r="F42" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="G42" s="34"/>
+      <c r="H42" s="34"/>
+      <c r="I42" s="34"/>
+    </row>
+    <row r="43" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B43" s="11">
+        <v>32</v>
+      </c>
+      <c r="C43" s="5">
+        <v>7508334.9506000001</v>
+      </c>
+      <c r="D43" s="5">
+        <v>4696769.0147000002</v>
+      </c>
+      <c r="E43" s="10">
+        <v>609.58299999999997</v>
+      </c>
+      <c r="F43" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="G43" s="34"/>
+      <c r="H43" s="34"/>
+      <c r="I43" s="34"/>
+    </row>
+    <row r="44" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B44" s="11">
+        <v>33</v>
+      </c>
+      <c r="C44" s="5">
+        <v>7508336.3622000003</v>
+      </c>
+      <c r="D44" s="5">
+        <v>4696769.9818000002</v>
+      </c>
+      <c r="E44" s="10">
+        <v>609.58299999999997</v>
+      </c>
+      <c r="F44" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="G44" s="34"/>
+      <c r="H44" s="34"/>
+      <c r="I44" s="34"/>
+    </row>
+    <row r="45" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B45" s="11">
+        <v>34</v>
+      </c>
+      <c r="C45" s="5">
+        <v>7508336.6776999999</v>
+      </c>
+      <c r="D45" s="5">
+        <v>4696769.9379000003</v>
+      </c>
+      <c r="E45" s="10">
+        <v>609.58299999999997</v>
+      </c>
+      <c r="F45" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="G45" s="34"/>
+      <c r="H45" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="I45" s="10">
+        <v>6.1769999999999996</v>
+      </c>
+    </row>
+    <row r="46" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B46" s="11">
+        <v>14</v>
+      </c>
+      <c r="C46" s="5">
+        <v>7508327.4062999999</v>
+      </c>
+      <c r="D46" s="5">
+        <v>4696770.5133999996</v>
+      </c>
+      <c r="E46" s="10">
+        <v>609.58299999999997</v>
+      </c>
+      <c r="F46" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="G39" s="26"/>
-      <c r="H39" s="15" t="s">
+      <c r="G46" s="34"/>
+      <c r="H46" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="I39" s="15">
-        <f>SUM(I33:I38)</f>
-        <v>83.265000000000001</v>
-      </c>
-    </row>
-    <row r="40" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="D40" s="6"/>
-      <c r="E40" s="7"/>
-      <c r="F40" s="7"/>
-      <c r="G40" s="8"/>
-      <c r="H40" s="9"/>
-      <c r="I40" s="9"/>
-    </row>
-    <row r="41" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="D41" s="6"/>
-      <c r="E41" s="7"/>
-      <c r="F41" s="7"/>
-      <c r="G41" s="8"/>
-      <c r="H41" s="9"/>
-      <c r="I41" s="9"/>
-    </row>
-    <row r="42" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="D42" s="6"/>
-      <c r="E42" s="7"/>
-      <c r="F42" s="7"/>
-      <c r="G42" s="8"/>
-      <c r="H42" s="9"/>
-      <c r="I42" s="9"/>
-    </row>
-    <row r="43" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="D43" s="6"/>
-      <c r="E43" s="7"/>
-      <c r="F43" s="7"/>
-      <c r="G43" s="8"/>
-      <c r="H43" s="9"/>
-      <c r="I43" s="9"/>
-    </row>
-    <row r="44" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="D44" s="6"/>
-      <c r="E44" s="7"/>
-      <c r="F44" s="7"/>
-      <c r="G44" s="8"/>
-      <c r="H44" s="9"/>
-      <c r="I44" s="9"/>
-    </row>
-    <row r="45" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="D45" s="6"/>
-      <c r="E45" s="7"/>
-      <c r="F45" s="7"/>
-      <c r="G45" s="8"/>
-      <c r="H45" s="9"/>
-      <c r="I45" s="9"/>
-    </row>
-    <row r="46" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="D46" s="6"/>
-      <c r="E46" s="7"/>
-      <c r="F46" s="7"/>
-      <c r="G46" s="8"/>
-      <c r="H46" s="9"/>
-      <c r="I46" s="9"/>
+      <c r="I46" s="15">
+        <f>SUM(I33:I45)</f>
+        <v>94.042000000000002</v>
+      </c>
     </row>
     <row r="47" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D47" s="6"/>
@@ -1998,79 +2087,138 @@
       <c r="I51" s="9"/>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B52" s="12"/>
-      <c r="C52" s="12"/>
       <c r="D52" s="6"/>
       <c r="E52" s="7"/>
       <c r="F52" s="7"/>
       <c r="G52" s="8"/>
-      <c r="H52" s="13"/>
-      <c r="I52" s="13"/>
-    </row>
-    <row r="53" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="K53" s="1"/>
-    </row>
-    <row r="54" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A54" s="2" t="s">
+      <c r="H52" s="9"/>
+      <c r="I52" s="9"/>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D53" s="6"/>
+      <c r="E53" s="7"/>
+      <c r="F53" s="7"/>
+      <c r="G53" s="8"/>
+      <c r="H53" s="9"/>
+      <c r="I53" s="9"/>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D54" s="6"/>
+      <c r="E54" s="7"/>
+      <c r="F54" s="7"/>
+      <c r="G54" s="8"/>
+      <c r="H54" s="9"/>
+      <c r="I54" s="9"/>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D55" s="6"/>
+      <c r="E55" s="7"/>
+      <c r="F55" s="7"/>
+      <c r="G55" s="8"/>
+      <c r="H55" s="9"/>
+      <c r="I55" s="9"/>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D56" s="6"/>
+      <c r="E56" s="7"/>
+      <c r="F56" s="7"/>
+      <c r="G56" s="8"/>
+      <c r="H56" s="9"/>
+      <c r="I56" s="9"/>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D57" s="6"/>
+      <c r="E57" s="7"/>
+      <c r="F57" s="7"/>
+      <c r="G57" s="8"/>
+      <c r="H57" s="9"/>
+      <c r="I57" s="9"/>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D58" s="6"/>
+      <c r="E58" s="7"/>
+      <c r="F58" s="7"/>
+      <c r="G58" s="8"/>
+      <c r="H58" s="9"/>
+      <c r="I58" s="9"/>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B59" s="12"/>
+      <c r="C59" s="12"/>
+      <c r="D59" s="6"/>
+      <c r="E59" s="7"/>
+      <c r="F59" s="7"/>
+      <c r="G59" s="8"/>
+      <c r="H59" s="13"/>
+      <c r="I59" s="13"/>
+    </row>
+    <row r="60" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="K60" s="1"/>
+    </row>
+    <row r="61" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A61" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B54" s="3"/>
-      <c r="C54" s="3"/>
-      <c r="D54" s="3"/>
-      <c r="E54" s="36" t="s">
+      <c r="B61" s="3"/>
+      <c r="C61" s="3"/>
+      <c r="D61" s="3"/>
+      <c r="E61" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="F54" s="37"/>
-      <c r="G54" s="38"/>
-      <c r="H54" s="32" t="s">
+      <c r="F61" s="26"/>
+      <c r="G61" s="27"/>
+      <c r="H61" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="I54" s="33"/>
-      <c r="J54" s="27"/>
-      <c r="K54" s="28"/>
-    </row>
-    <row r="55" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A55" s="39" t="s">
+      <c r="I61" s="22"/>
+      <c r="J61" s="16"/>
+      <c r="K61" s="17"/>
+    </row>
+    <row r="62" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A62" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="B55" s="40"/>
-      <c r="C55" s="40"/>
-      <c r="D55" s="41"/>
-      <c r="E55" s="42">
+      <c r="B62" s="29"/>
+      <c r="C62" s="29"/>
+      <c r="D62" s="30"/>
+      <c r="E62" s="31">
         <v>140</v>
       </c>
-      <c r="F55" s="43"/>
-      <c r="G55" s="44"/>
-      <c r="H55" s="34"/>
-      <c r="I55" s="35"/>
-      <c r="J55" s="29"/>
-      <c r="K55" s="30"/>
-    </row>
-    <row r="56" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="K56" s="1"/>
-    </row>
-    <row r="57" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="K57" s="1"/>
-    </row>
-    <row r="58" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="K58" s="1"/>
+      <c r="F62" s="32"/>
+      <c r="G62" s="33"/>
+      <c r="H62" s="23"/>
+      <c r="I62" s="24"/>
+      <c r="J62" s="18"/>
+      <c r="K62" s="19"/>
+    </row>
+    <row r="63" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="K63" s="1"/>
+    </row>
+    <row r="64" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="K64" s="1"/>
+    </row>
+    <row r="65" spans="11:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="K65" s="1"/>
     </row>
   </sheetData>
+  <sortState ref="N23:N24">
+    <sortCondition ref="N25"/>
+  </sortState>
   <mergeCells count="14">
-    <mergeCell ref="J54:K55"/>
-    <mergeCell ref="A3:K6"/>
-    <mergeCell ref="H54:I55"/>
-    <mergeCell ref="E54:G54"/>
-    <mergeCell ref="A55:D55"/>
-    <mergeCell ref="E55:G55"/>
-    <mergeCell ref="G33:G39"/>
-    <mergeCell ref="H33:H37"/>
-    <mergeCell ref="I33:I37"/>
-    <mergeCell ref="H15:H28"/>
-    <mergeCell ref="I15:I28"/>
     <mergeCell ref="A1:K2"/>
     <mergeCell ref="C8:J10"/>
     <mergeCell ref="G15:G29"/>
+    <mergeCell ref="J61:K62"/>
+    <mergeCell ref="A3:K6"/>
+    <mergeCell ref="H61:I62"/>
+    <mergeCell ref="E61:G61"/>
+    <mergeCell ref="A62:D62"/>
+    <mergeCell ref="E62:G62"/>
+    <mergeCell ref="G33:G46"/>
+    <mergeCell ref="H33:H44"/>
+    <mergeCell ref="I33:I44"/>
+    <mergeCell ref="H15:H28"/>
+    <mergeCell ref="I15:I28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="58" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>